<commit_message>
change tracing strategy and save wallet labels
</commit_message>
<xml_diff>
--- a/data/token/BTC.xlsx
+++ b/data/token/BTC.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -86,6 +86,12 @@
   </si>
   <si>
     <t>2024-08-31</t>
+  </si>
+  <si>
+    <t>2024-10-04</t>
+  </si>
+  <si>
+    <t>2024-10-03</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -633,6 +639,22 @@
         <v>59129.05</v>
       </c>
     </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>60746.35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>60641.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>